<commit_message>
Updating Self Learning Test Cases & Results
</commit_message>
<xml_diff>
--- a/Self_Learning_Testcases_and_Results/Self Learning Test Case Results.xlsx
+++ b/Self_Learning_Testcases_and_Results/Self Learning Test Case Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\Class12Capstone\Self_Learning_Testcases_and_Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43CB240A-80ED-4D26-A5A9-7B1FBCAC197A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A63DA70-23BA-4910-8447-B6DD07B072F4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3EAA6031-D306-4FED-90EA-377CB01D9B4F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{3EAA6031-D306-4FED-90EA-377CB01D9B4F}"/>
   </bookViews>
   <sheets>
     <sheet name="Self Learning TC1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="25">
   <si>
     <t>Assumptions:</t>
   </si>
@@ -84,9 +84,6 @@
     <t xml:space="preserve">Nmap should populate detailed information on the website you scanned showing you the actively open ports as well as the traceroutes discovered within the Ipaddress.  </t>
   </si>
   <si>
-    <t xml:space="preserve">Nmap should populate a list of the open ports located through the Ipaddress you scanned. Take note of which ports are open. Port 443/tcp mysql is a commonly targeted port by hackers. You should take measure to ensure that these ports is properly secured. </t>
-  </si>
-  <si>
     <t xml:space="preserve">3. On the right side of the application ensure "Quick Scan" is selected as the profile option and then click the "Scan" commmand. </t>
   </si>
   <si>
@@ -97,6 +94,21 @@
   </si>
   <si>
     <t>PASS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Take note of which ports are open. Port 443/tcp mysql is a commonly targeted port by hackers. You should take measure to ensure that this port is properly secured. </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Traceroutes should be located near the bottom of the scan showing you a list of Ip addresses and the name of routers that the packet information is passing through.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nmap should populate a list of the open ports located through the Ipaddress you scanned. </t>
+  </si>
+  <si>
+    <t>INCONCLUSIVE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4. Scroll down the information to find the traceroutes. </t>
   </si>
 </sst>
 </file>
@@ -237,7 +249,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -264,6 +276,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -584,8 +599,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D76EB1B-99AF-4FFC-9D69-7334799D424F}">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11:C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -669,17 +684,21 @@
       <c r="B13" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C13" s="12" t="s">
         <v>15</v>
       </c>
       <c r="D13" s="7"/>
       <c r="E13" s="7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="11"/>
-      <c r="C14" s="11"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="44.4" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>21</v>
+      </c>
       <c r="D14" s="7"/>
       <c r="E14" s="7"/>
     </row>
@@ -713,8 +732,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C85EA735-9174-4AB5-8C63-76369BCF6C20}">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11:C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -722,8 +741,8 @@
     <col min="1" max="1" width="55.44140625" customWidth="1"/>
     <col min="2" max="2" width="49.5546875" customWidth="1"/>
     <col min="3" max="3" width="53.6640625" customWidth="1"/>
-    <col min="4" max="4" width="19.33203125" customWidth="1"/>
-    <col min="5" max="5" width="13.21875" customWidth="1"/>
+    <col min="4" max="4" width="27.109375" customWidth="1"/>
+    <col min="5" max="5" width="17.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -746,7 +765,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -771,7 +790,7 @@
     </row>
     <row r="11" spans="1:5" ht="75.599999999999994" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>9</v>
@@ -794,14 +813,16 @@
     <row r="13" spans="1:5" ht="85.2" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="10"/>
       <c r="B13" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="D13" s="7"/>
+        <v>22</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>20</v>
+      </c>
       <c r="E13" s="7" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">

</xml_diff>